<commit_message>
Updates to task list, initial commit of pwm with serial program (working)
</commit_message>
<xml_diff>
--- a/Documentation/Project Management/Task List.xlsx
+++ b/Documentation/Project Management/Task List.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\ELEC4850\Part A\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Willie\Documents\Uni\Newcastle\4 Fourth Year\1 Final Year Project\trunk\Documentation\Project Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D83E1730-B599-4135-AAF7-F6D680EB3F39}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
   <si>
     <t>Task List</t>
   </si>
@@ -96,12 +97,42 @@
   </si>
   <si>
     <t>Benefits</t>
+  </si>
+  <si>
+    <t>Predecessor</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>1 - 5</t>
+  </si>
+  <si>
+    <t>4, 11</t>
+  </si>
+  <si>
+    <t>4, 11, 17</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Difficulty (/10)</t>
+  </si>
+  <si>
+    <t>5 - 10</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -146,10 +177,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,133 +480,342 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:B28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="57" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="8" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="C4" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="C5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="C6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="C7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="C8" s="4">
+        <v>3</v>
+      </c>
+      <c r="D8" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>5</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="C9" s="4">
+        <v>2</v>
+      </c>
+      <c r="D9" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
+      <c r="C10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+      <c r="C12" s="4"/>
+      <c r="D12" s="5"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+      <c r="B13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>8</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+      <c r="C14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>9</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+      <c r="C15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>10</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+      <c r="C16" s="4">
+        <v>17</v>
+      </c>
+      <c r="D16" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>11</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+      <c r="C17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>12</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+      <c r="C18" s="4">
+        <v>17</v>
+      </c>
+      <c r="D18" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>13</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+      <c r="C19" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>14</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+      <c r="C20" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>15</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+      <c r="C21" s="4">
+        <v>14</v>
+      </c>
+      <c r="D21" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>16</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="2" t="s">
+      <c r="C22" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="5"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+      <c r="C24" s="4"/>
+      <c r="D24" s="5"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>17</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+      <c r="C25" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>18</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+      <c r="C26" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>19</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+      <c r="C27" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>20</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>23</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>